<commit_message>
ng: add koji survey
</commit_message>
<xml_diff>
--- a/ONCHO/Entomological survey Survey/Nigeria/2023/dec/ng_oncho_bsc_202312_capture_koji.xlsx
+++ b/ONCHO/Entomological survey Survey/Nigeria/2023/dec/ng_oncho_bsc_202312_capture_koji.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2023\dec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449B90EF-49CF-4381-BCD3-5B16D91906C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E5CB10-6124-4F79-8D38-0189031EA2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -350,12 +350,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>ss_2</t>
-  </si>
-  <si>
-    <t>ng_oncho_bsc_202312_capture_koji</t>
-  </si>
-  <si>
     <t>(2023 December) - Koji: Human Landing Catches</t>
   </si>
   <si>
@@ -660,6 +654,12 @@
   </si>
   <si>
     <t>KOG_OMA_M_045</t>
+  </si>
+  <si>
+    <t>ng_oncho_bsc_202312_capture_koji_v2</t>
+  </si>
+  <si>
+    <t>kj_2</t>
   </si>
 </sst>
 </file>
@@ -1099,11 +1099,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1415,7 +1415,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>105</v>
+        <v>208</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>41</v>
@@ -1626,7 +1626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A123" sqref="A123:A130"/>
     </sheetView>
@@ -1900,10 +1900,10 @@
         <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1911,13 +1911,13 @@
         <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1925,13 +1925,13 @@
         <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1939,13 +1939,13 @@
         <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1953,13 +1953,13 @@
         <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1967,13 +1967,13 @@
         <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1981,13 +1981,13 @@
         <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1995,13 +1995,13 @@
         <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2009,13 +2009,13 @@
         <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2023,13 +2023,13 @@
         <v>57</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -2037,13 +2037,13 @@
         <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2051,13 +2051,13 @@
         <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2065,13 +2065,13 @@
         <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2079,13 +2079,13 @@
         <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2093,13 +2093,13 @@
         <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D41" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2107,13 +2107,13 @@
         <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2121,13 +2121,13 @@
         <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2135,13 +2135,13 @@
         <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2149,13 +2149,13 @@
         <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2163,13 +2163,13 @@
         <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C47" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2177,13 +2177,13 @@
         <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C48" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E48" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2191,13 +2191,13 @@
         <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E49" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2205,13 +2205,13 @@
         <v>58</v>
       </c>
       <c r="B50" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C50" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2219,13 +2219,13 @@
         <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C51" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2233,13 +2233,13 @@
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C52" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E52" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2247,13 +2247,13 @@
         <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C53" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E53" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2261,13 +2261,13 @@
         <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C54" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E54" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2275,13 +2275,13 @@
         <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C55" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E55" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2289,13 +2289,13 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E56" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2303,13 +2303,13 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E57" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2317,13 +2317,13 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C58" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E58" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2331,13 +2331,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C59" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E59" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2345,13 +2345,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C60" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E60" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2359,13 +2359,13 @@
         <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C61" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E61" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2373,13 +2373,13 @@
         <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C62" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E62" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2387,13 +2387,13 @@
         <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C63" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E63" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2401,13 +2401,13 @@
         <v>58</v>
       </c>
       <c r="B64" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C64" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E64" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2415,13 +2415,13 @@
         <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C65" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E65" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2429,13 +2429,13 @@
         <v>58</v>
       </c>
       <c r="B66" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C66" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E66" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2443,13 +2443,13 @@
         <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C67" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E67" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2457,13 +2457,13 @@
         <v>58</v>
       </c>
       <c r="B68" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C68" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E68" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2471,13 +2471,13 @@
         <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C69" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E69" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2485,13 +2485,13 @@
         <v>58</v>
       </c>
       <c r="B70" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E70" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2499,13 +2499,13 @@
         <v>58</v>
       </c>
       <c r="B71" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C71" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E71" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2513,13 +2513,13 @@
         <v>58</v>
       </c>
       <c r="B72" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C72" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E72" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2527,13 +2527,13 @@
         <v>58</v>
       </c>
       <c r="B73" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C73" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E73" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2541,13 +2541,13 @@
         <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C74" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E74" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2555,13 +2555,13 @@
         <v>58</v>
       </c>
       <c r="B75" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C75" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E75" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2569,13 +2569,13 @@
         <v>58</v>
       </c>
       <c r="B76" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C76" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E76" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2583,13 +2583,13 @@
         <v>58</v>
       </c>
       <c r="B77" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C77" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E77" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2597,13 +2597,13 @@
         <v>58</v>
       </c>
       <c r="B78" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C78" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E78" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2611,13 +2611,13 @@
         <v>58</v>
       </c>
       <c r="B79" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C79" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E79" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2625,13 +2625,13 @@
         <v>58</v>
       </c>
       <c r="B80" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C80" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E80" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2639,13 +2639,13 @@
         <v>58</v>
       </c>
       <c r="B81" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C81" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E81" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2653,13 +2653,13 @@
         <v>58</v>
       </c>
       <c r="B82" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C82" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E82" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2667,13 +2667,13 @@
         <v>58</v>
       </c>
       <c r="B83" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C83" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E83" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2681,13 +2681,13 @@
         <v>58</v>
       </c>
       <c r="B84" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C84" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E84" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2695,13 +2695,13 @@
         <v>94</v>
       </c>
       <c r="B86" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C86" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2709,13 +2709,13 @@
         <v>94</v>
       </c>
       <c r="B87" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C87" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F87" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2723,13 +2723,13 @@
         <v>94</v>
       </c>
       <c r="B88" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C88" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F88" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2737,13 +2737,13 @@
         <v>94</v>
       </c>
       <c r="B89" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C89" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F89" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2751,13 +2751,13 @@
         <v>94</v>
       </c>
       <c r="B90" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C90" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F90" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2765,13 +2765,13 @@
         <v>94</v>
       </c>
       <c r="B91" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C91" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F91" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2779,13 +2779,13 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C92" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F92" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2793,13 +2793,13 @@
         <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C93" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F93" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2807,13 +2807,13 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C94" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F94" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2821,13 +2821,13 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C95" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F95" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2835,13 +2835,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C96" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F96" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2849,13 +2849,13 @@
         <v>94</v>
       </c>
       <c r="B97" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C97" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F97" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2863,13 +2863,13 @@
         <v>94</v>
       </c>
       <c r="B98" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C98" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F98" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2877,13 +2877,13 @@
         <v>94</v>
       </c>
       <c r="B99" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C99" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F99" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2891,13 +2891,13 @@
         <v>94</v>
       </c>
       <c r="B100" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C100" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F100" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2905,13 +2905,13 @@
         <v>94</v>
       </c>
       <c r="B101" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C101" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F101" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2919,13 +2919,13 @@
         <v>94</v>
       </c>
       <c r="B102" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C102" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F102" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2933,13 +2933,13 @@
         <v>94</v>
       </c>
       <c r="B103" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C103" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F103" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2947,13 +2947,13 @@
         <v>94</v>
       </c>
       <c r="B104" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C104" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F104" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2961,13 +2961,13 @@
         <v>94</v>
       </c>
       <c r="B105" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C105" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F105" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2975,13 +2975,13 @@
         <v>94</v>
       </c>
       <c r="B106" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C106" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F106" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2989,13 +2989,13 @@
         <v>94</v>
       </c>
       <c r="B107" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C107" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F107" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -3003,13 +3003,13 @@
         <v>94</v>
       </c>
       <c r="B108" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C108" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F108" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -3017,13 +3017,13 @@
         <v>94</v>
       </c>
       <c r="B109" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C109" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F109" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3031,13 +3031,13 @@
         <v>94</v>
       </c>
       <c r="B110" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C110" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F110" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -3045,13 +3045,13 @@
         <v>94</v>
       </c>
       <c r="B111" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C111" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F111" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3059,13 +3059,13 @@
         <v>94</v>
       </c>
       <c r="B112" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C112" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F112" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3073,13 +3073,13 @@
         <v>94</v>
       </c>
       <c r="B113" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C113" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F113" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3087,13 +3087,13 @@
         <v>94</v>
       </c>
       <c r="B114" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C114" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F114" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3101,13 +3101,13 @@
         <v>94</v>
       </c>
       <c r="B115" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C115" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F115" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -3115,13 +3115,13 @@
         <v>94</v>
       </c>
       <c r="B116" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C116" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F116" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -3129,13 +3129,13 @@
         <v>94</v>
       </c>
       <c r="B117" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C117" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F117" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3143,13 +3143,13 @@
         <v>94</v>
       </c>
       <c r="B118" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C118" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F118" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -3157,13 +3157,13 @@
         <v>94</v>
       </c>
       <c r="B119" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C119" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F119" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3171,13 +3171,13 @@
         <v>94</v>
       </c>
       <c r="B120" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C120" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F120" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -3185,13 +3185,13 @@
         <v>94</v>
       </c>
       <c r="B121" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C121" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F121" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -3199,13 +3199,13 @@
         <v>94</v>
       </c>
       <c r="B122" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C122" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F122" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3213,13 +3213,13 @@
         <v>94</v>
       </c>
       <c r="B123" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C123" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F123" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -3227,13 +3227,13 @@
         <v>94</v>
       </c>
       <c r="B124" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C124" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F124" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3241,13 +3241,13 @@
         <v>94</v>
       </c>
       <c r="B125" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C125" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F125" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3255,13 +3255,13 @@
         <v>94</v>
       </c>
       <c r="B126" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C126" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F126" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3269,13 +3269,13 @@
         <v>94</v>
       </c>
       <c r="B127" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C127" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F127" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3283,13 +3283,13 @@
         <v>94</v>
       </c>
       <c r="B128" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C128" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F128" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -3297,13 +3297,13 @@
         <v>94</v>
       </c>
       <c r="B129" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C129" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F129" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3311,13 +3311,13 @@
         <v>94</v>
       </c>
       <c r="B130" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C130" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F130" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3334,7 +3334,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3356,10 +3356,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>106</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
         <v>80</v>

</xml_diff>